<commit_message>
ordenamientos recursivos arr, tests pendientes
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 5.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 5.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lina/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Documents\Uniandes\EDA\Reestructura\ISIS1225-Laboratorio-5\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6DE5ECC-B753-4C4F-8EF0-1FF87AB8F3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C077633-6DB4-480A-8DD5-0CF440602032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-26970" yWindow="2115" windowWidth="21600" windowHeight="11295" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="01-Data Lab 4" sheetId="1" r:id="rId1"/>
     <sheet name="02-Insertion Sort" sheetId="8" r:id="rId2"/>
     <sheet name="03-Selection Sort" sheetId="14" r:id="rId3"/>
     <sheet name="04-Shell Sort" sheetId="26" r:id="rId4"/>
+    <sheet name="05-Merge Sort" sheetId="27" r:id="rId5"/>
+    <sheet name="06-Quick Sort" sheetId="28" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,8 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>Porcentaje de la muestra [pct]</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>TIEMPOS DE EJECUCIÓN SHELL SORT[ms]</t>
+  </si>
+  <si>
+    <t>TIEMPOS DE EJECUCIÓN MERGE SORT[ms]</t>
+  </si>
+  <si>
+    <t>TIEMPOS DE EJECUCIÓN QUICK SORT[ms]</t>
   </si>
 </sst>
 </file>
@@ -124,7 +130,7 @@
       <name val="Dax-Regular"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +158,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC1F8F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2B2E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAB0AA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -309,17 +327,11 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -339,9 +351,6 @@
     <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -352,6 +361,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -381,26 +402,29 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="25">
     <dxf>
       <font>
         <b/>
@@ -445,6 +469,104 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -593,6 +715,196 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -709,6 +1021,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEAB0AA"/>
+      <color rgb="FFE2B2E3"/>
       <color rgb="FFC1F8F3"/>
       <color rgb="FF7FF9EA"/>
       <color rgb="FF73FDD6"/>
@@ -796,7 +1110,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -889,7 +1203,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1026,7 +1340,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1168,7 +1482,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1206,7 +1520,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -1285,7 +1599,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1323,7 +1637,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -1365,7 +1679,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1402,7 +1716,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1481,7 +1795,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1574,7 +1888,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1711,7 +2025,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1853,7 +2167,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1891,7 +2205,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -1970,7 +2284,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2008,7 +2322,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2050,7 +2364,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2087,7 +2401,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2163,7 +2477,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2256,7 +2570,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2393,7 +2707,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2535,7 +2849,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2573,7 +2887,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2652,7 +2966,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2690,7 +3004,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2732,7 +3046,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2769,7 +3083,1371 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Comparación de tiempos de ejecucion Merge</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> Sort</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'01-Data Lab 4'!$H$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Array List</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1363811854896437"/>
+                  <c:y val="-3.2945200031814204E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$F$14:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$H$14:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FBFE-4DE8-B6E0-DE4FEFDE004A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'01-Data Lab 4'!$I$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linked List</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.593553005287829E-2"/>
+                  <c:y val="0.12376727909011373"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$F$14:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$I$14:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FBFE-4DE8-B6E0-DE4FEFDE004A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1328118000"/>
+        <c:axId val="1328121328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1328118000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Tamaño</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> de la muestra [Num. elementos]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1328121328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1328121328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Tiempo de Ejecución [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1328118000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Comparación de tiempos de ejecucion Quick</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> Sort</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'01-Data Lab 4'!$C$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Array List</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1363811854896437"/>
+                  <c:y val="-3.2945200031814204E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$A$25:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$C$25:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0E3F-4D83-B3F0-06019FFE22C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'01-Data Lab 4'!$D$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linked List</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.593553005287829E-2"/>
+                  <c:y val="0.12376727909011373"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$A$25:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$D$25:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0E3F-4D83-B3F0-06019FFE22C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1328118000"/>
+        <c:axId val="1328121328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1328118000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Tamaño</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> de la muestra [Num. elementos]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1328121328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1328121328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Tiempo de Ejecución [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1328118000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2895,6 +4573,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3928,6 +5686,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4482,11 +7272,37 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D61CD20E-8C47-43B3-BEC2-00339C536135}">
+  <sheetPr>
+    <tabColor rgb="FFE2B2E3"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0DB576FC-CFC3-493F-9CD6-9BF52318F22D}">
+  <sheetPr>
+    <tabColor rgb="FFEAB0AA"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8674100" cy="6286500"/>
+    <xdr:ext cx="8667750" cy="6296025"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4519,7 +7335,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8674100" cy="6286500"/>
+    <xdr:ext cx="8667750" cy="6296025"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4552,7 +7368,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8674100" cy="6286500"/>
+    <xdr:ext cx="8667750" cy="6296025"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -4581,8 +7397,74 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37CAA8E9-5D32-43B0-9370-53D61A8522F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D024CFB-96DA-4763-A702-F3EB8C939D2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:D10" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:D10" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="A2:D10" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4590,19 +7472,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Porcentaje de la muestra [pct]" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tamaño de la muestra (ARRAY_LIST)" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Porcentaje de la muestra [pct]" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tamaño de la muestra (ARRAY_LIST)" dataDxfId="20">
       <calculatedColumnFormula>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Array List" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Linked List" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Array List" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Linked List" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A13:D21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A13:D21" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A13:D21" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4610,21 +7492,51 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Porcentaje de la muestra [pct]" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Porcentaje de la muestra [pct]" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="14">
       <calculatedColumnFormula>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Array List" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Linked List" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Array List" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Linked List" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{87C8722B-DD68-4653-A5A0-21E5FA4E5167}" name="Table134" displayName="Table134" ref="F13:I21" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="F13:I21" xr:uid="{87C8722B-DD68-4653-A5A0-21E5FA4E5167}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C07ABC3E-F8C1-4672-A7B8-F11CF0E5A083}" name="Porcentaje de la muestra [pct]" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{4E1C97DA-811C-4F4D-AD84-0E8397D4D278}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="8">
+      <calculatedColumnFormula>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{699BF631-EF19-4B17-9C43-D855DD8713A3}" name="Array List" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{F753368E-60C6-4559-AAB2-8D5D39D13D08}" name="Linked List" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{35AE231F-BBB3-413D-8E8D-6DED34128222}" name="Table135" displayName="Table135" ref="A24:D32" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A24:D32" xr:uid="{35AE231F-BBB3-413D-8E8D-6DED34128222}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3AE7D498-7B8C-404E-94ED-AC1F2545D8BA}" name="Porcentaje de la muestra [pct]" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{8889E6E7-DD99-4C87-ADCA-7FD6746EF539}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="2">
+      <calculatedColumnFormula>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{996BC463-8C92-4516-B4BC-F2A077D7A2EF}" name="Array List" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{6921D7A0-1F93-44BF-B532-EF08353E773B}" name="Linked List" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4662,7 +7574,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4768,7 +7680,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4910,7 +7822,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4918,37 +7830,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C25" sqref="C25:D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" style="3" customWidth="1"/>
-    <col min="6" max="12" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
+    <col min="6" max="12" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-      <c r="F1" s="27" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="F1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="33" thickBot="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="45.75" thickBot="1">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -4957,45 +7869,45 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B3" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14">
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="13">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>0.05</v>
       </c>
       <c r="B4" s="5">
@@ -5003,9 +7915,9 @@
         <v>500</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="8">
+      <c r="D4" s="14"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="7">
         <v>0.05</v>
       </c>
       <c r="G4" s="5">
@@ -5013,31 +7925,31 @@
         <v>500</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="17"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>0.1</v>
       </c>
       <c r="B5" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14">
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12">
         <v>0.1</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="13">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>0.2</v>
       </c>
       <c r="B6" s="5">
@@ -5045,9 +7957,9 @@
         <v>2000</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="8">
+      <c r="D6" s="14"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="7">
         <v>0.2</v>
       </c>
       <c r="G6" s="5">
@@ -5055,31 +7967,31 @@
         <v>2000</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="17"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>0.3</v>
       </c>
       <c r="B7" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14">
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12">
         <v>0.3</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>0.5</v>
       </c>
       <c r="B8" s="5">
@@ -5087,9 +7999,9 @@
         <v>5000</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="8">
+      <c r="D8" s="14"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="7">
         <v>0.5</v>
       </c>
       <c r="G8" s="5">
@@ -5097,67 +8009,69 @@
         <v>5000</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="17"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>0.8</v>
       </c>
       <c r="B9" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14">
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12">
         <v>0.8</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="13">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="34"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="1:9" ht="16" thickBot="1">
-      <c r="A10" s="10">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A10" s="8">
         <v>1</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="9">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="10">
+      <c r="C10" s="10"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="8">
         <v>1</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="9">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="18"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="1:9" ht="16" thickBot="1">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
       <c r="E11"/>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
+      <c r="F12" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="32">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="30">
+      <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -5166,16 +8080,24 @@
       <c r="C13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="F13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B14" s="5">
@@ -5183,15 +8105,20 @@
         <v>50</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="9"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G14" s="5">
+        <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>50</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>0.05</v>
       </c>
       <c r="B15" s="5">
@@ -5199,15 +8126,20 @@
         <v>500</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="9"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="G15" s="5">
+        <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>500</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>0.1</v>
       </c>
       <c r="B16" s="5">
@@ -5215,15 +8147,20 @@
         <v>1000</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="9"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G16" s="5">
+        <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>1000</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>0.2</v>
       </c>
       <c r="B17" s="5">
@@ -5231,15 +8168,20 @@
         <v>2000</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="9"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="5">
+        <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>2000</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="8">
+      <c r="A18" s="7">
         <v>0.3</v>
       </c>
       <c r="B18" s="5">
@@ -5247,15 +8189,20 @@
         <v>3000</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="9"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G18" s="5">
+        <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>3000</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="8">
+      <c r="A19" s="7">
         <v>0.5</v>
       </c>
       <c r="B19" s="5">
@@ -5263,15 +8210,20 @@
         <v>5000</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="9"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G19" s="5">
+        <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>5000</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="8">
+      <c r="A20" s="7">
         <v>0.8</v>
       </c>
       <c r="B20" s="5">
@@ -5279,46 +8231,292 @@
         <v>8000</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="9"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="G20" s="5">
+        <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>8000</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="14"/>
     </row>
-    <row r="21" spans="1:9" ht="16" thickBot="1">
-      <c r="A21" s="10">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A21" s="8">
         <v>1</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="9">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="8">
+        <v>1</v>
+      </c>
+      <c r="G21" s="9">
+        <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>10000</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1"/>
+    <row r="23" spans="1:9">
+      <c r="A23" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="36"/>
+    </row>
+    <row r="24" spans="1:9" ht="30">
+      <c r="A24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B25" s="5">
+        <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>50</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="B26" s="5">
+        <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>500</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="B27" s="5">
+        <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>1000</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="B28" s="5">
+        <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>2000</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="B29" s="5">
+        <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>3000</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="B30" s="5">
+        <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>5000</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="14"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="B31" s="5">
+        <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>8000</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="14"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A32" s="8">
+        <v>1</v>
+      </c>
+      <c r="B32" s="9">
+        <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>10000</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F12:I12"/>
+    <mergeCell ref="A23:D23"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
+      <UserInfo>
+        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Arturo Henao Chaparro</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
+        <AccountId>52</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan Carlos Marin Morales</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sofia Duque Gomez</DisplayName>
+        <AccountId>60</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Andres Felipe Romero Brand</DisplayName>
+        <AccountId>91</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
+        <AccountId>92</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
+        <AccountId>94</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan David Diaz Ipuz</DisplayName>
+        <AccountId>90</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Isaac David Bermudez Lara</DisplayName>
+        <AccountId>95</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
+        <AccountId>55</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
+        <AccountId>97</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kevin Cohen Solano</DisplayName>
+        <AccountId>93</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
+        <AccountId>96</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4e7eefc5f66e7d51449543297ddde059">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df8efc3b1b447b14ec56bc155bd746d7" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -5567,143 +8765,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
-      <UserInfo>
-        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Arturo Henao Chaparro</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
-        <AccountId>52</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan Carlos Marin Morales</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sofia Duque Gomez</DisplayName>
-        <AccountId>60</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Andres Felipe Romero Brand</DisplayName>
-        <AccountId>91</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
-        <AccountId>92</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
-        <AccountId>94</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan David Diaz Ipuz</DisplayName>
-        <AccountId>90</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Isaac David Bermudez Lara</DisplayName>
-        <AccountId>95</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
-        <AccountId>55</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
-        <AccountId>97</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kevin Cohen Solano</DisplayName>
-        <AccountId>93</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
-        <AccountId>96</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BEEE7F2-DD9A-42EF-8F73-A92FC7ED8D52}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5726,9 +8791,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BEEE7F2-DD9A-42EF-8F73-A92FC7ED8D52}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Llamada de funciones y array list excel
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 5.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Documents\Uniandes\EDA\Reestructura\ISIS1225-Laboratorio-5\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aef29e720c6d702c/Desktop/UNIANDES/Trabajos/Pregrado/Segundo Semestre/EDA/Laboratorio5-G03/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C077633-6DB4-480A-8DD5-0CF440602032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{8C077633-6DB4-480A-8DD5-0CF440602032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4400350D-8F77-4424-8102-88A1A1704D5A}"/>
   <bookViews>
-    <workbookView xWindow="-26970" yWindow="2115" windowWidth="21600" windowHeight="11295" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="01-Data Lab 4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>Porcentaje de la muestra [pct]</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>TIEMPOS DE EJECUCIÓN QUICK SORT[ms]</t>
+  </si>
+  <si>
+    <t>0.995</t>
+  </si>
+  <si>
+    <t>0.760</t>
   </si>
 </sst>
 </file>
@@ -314,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -338,9 +344,6 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -367,9 +370,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -419,6 +419,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1110,7 +1119,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1245,8 +1254,32 @@
             <c:numRef>
               <c:f>'01-Data Lab 4'!$C$3:$C$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1072</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115264</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>273724</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1123871</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3523236</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6549118</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18359474</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34499564</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1482,7 +1515,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1603,7 +1636,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1930,8 +1963,32 @@
             <c:numRef>
               <c:f>'01-Data Lab 4'!$C$14:$C$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1638</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>136477</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>394010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1124549</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2489934</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7000043</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29702695</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40013216</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2167,7 +2224,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2288,7 +2345,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2477,7 +2534,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2612,8 +2669,32 @@
             <c:numRef>
               <c:f>'01-Data Lab 4'!$H$3:$H$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1775</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>388982</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1018589</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2231269</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6582562</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18741444</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38876693</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2849,7 +2930,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2970,7 +3051,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3159,7 +3240,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3294,8 +3375,32 @@
             <c:numRef>
               <c:f>'01-Data Lab 4'!$H$14:$H$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77611</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>280858</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>812573</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2112914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5762327</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16584472</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31087177</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3531,7 +3636,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3841,7 +3946,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3976,8 +4081,32 @@
             <c:numRef>
               <c:f>'01-Data Lab 4'!$C$25:$C$32</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88084</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>237313</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>739908</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1798397</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6214284</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16625954</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31445595</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4213,7 +4342,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7239,7 +7368,7 @@
     <tabColor rgb="FFC1F8F3"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="55" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7252,7 +7381,7 @@
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="55" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7265,7 +7394,7 @@
     <tabColor rgb="FFF69E76"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="55" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7278,7 +7407,7 @@
     <tabColor rgb="FFE2B2E3"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="55" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7291,7 +7420,7 @@
     <tabColor rgb="FFEAB0AA"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="55" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7302,7 +7431,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7335,7 +7464,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7368,7 +7497,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -7401,7 +7530,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -7434,7 +7563,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -7534,9 +7663,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7574,7 +7703,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -7680,7 +7809,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7822,7 +7951,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7832,34 +7961,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:D32"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
-    <col min="6" max="12" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" style="3" customWidth="1"/>
+    <col min="6" max="12" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="F1" s="28" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="F1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="45.75" thickBot="1">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="42.5" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -7869,23 +7998,23 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="14">
       <c r="A3" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -7893,20 +8022,24 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12">
+      <c r="C3" s="37">
+        <v>1072</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
+      <c r="H3" s="37">
+        <v>1775</v>
+      </c>
+      <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="14">
       <c r="A4" s="7">
         <v>0.05</v>
       </c>
@@ -7914,9 +8047,11 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>500</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="11"/>
+      <c r="C4" s="35">
+        <v>115264</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="7">
         <v>0.05</v>
       </c>
@@ -7924,8 +8059,10 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>500</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="14"/>
+      <c r="H4" s="35">
+        <v>86800</v>
+      </c>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="7">
@@ -7935,18 +8072,22 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12">
+      <c r="C5" s="37">
+        <v>273724</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11">
         <v>0.1</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21"/>
+      <c r="H5" s="37">
+        <v>388982</v>
+      </c>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="7">
@@ -7956,9 +8097,11 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>2000</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="11"/>
+      <c r="C6" s="35">
+        <v>1123871</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="7">
         <v>0.2</v>
       </c>
@@ -7966,8 +8109,10 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>2000</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="14"/>
+      <c r="H6" s="35">
+        <v>1018589</v>
+      </c>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="7">
@@ -7977,18 +8122,22 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12">
+      <c r="C7" s="37">
+        <v>3523236</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11">
         <v>0.3</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
+      <c r="H7" s="37">
+        <v>2231269</v>
+      </c>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="7">
@@ -7998,9 +8147,11 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>5000</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="11"/>
+      <c r="C8" s="35">
+        <v>6549118</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="7">
         <v>0.5</v>
       </c>
@@ -8008,8 +8159,10 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>5000</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="14"/>
+      <c r="H8" s="35">
+        <v>6582562</v>
+      </c>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="7">
@@ -8019,20 +8172,24 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12">
+      <c r="C9" s="37">
+        <v>18359474</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11">
         <v>0.8</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
+      <c r="H9" s="37">
+        <v>18741444</v>
+      </c>
+      <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+    <row r="10" spans="1:9" ht="15" thickBot="1">
       <c r="A10" s="8">
         <v>1</v>
       </c>
@@ -8040,9 +8197,11 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="11"/>
+      <c r="C10" s="36">
+        <v>34499564</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="8">
         <v>1</v>
       </c>
@@ -8050,27 +8209,29 @@
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="15"/>
+      <c r="H10" s="36">
+        <v>38876693</v>
+      </c>
+      <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15" thickBot="1">
       <c r="E11"/>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="F12" s="31" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
+      <c r="F12" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31"/>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="30">
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="28">
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
@@ -8080,7 +8241,7 @@
       <c r="C13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -8092,11 +8253,11 @@
       <c r="H13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1">
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="14">
       <c r="A14" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -8104,9 +8265,11 @@
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="11"/>
+      <c r="C14" s="35">
+        <v>1638</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -8114,10 +8277,12 @@
         <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="14"/>
+      <c r="H14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1">
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="14">
       <c r="A15" s="7">
         <v>0.05</v>
       </c>
@@ -8125,9 +8290,11 @@
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>500</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="11"/>
+      <c r="C15" s="35">
+        <v>136477</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="7">
         <v>0.05</v>
       </c>
@@ -8135,8 +8302,10 @@
         <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>500</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="14"/>
+      <c r="H15" s="35">
+        <v>77611</v>
+      </c>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="7">
@@ -8146,9 +8315,11 @@
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="11"/>
+      <c r="C16" s="35">
+        <v>394010</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="7">
         <v>0.1</v>
       </c>
@@ -8156,8 +8327,10 @@
         <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="14"/>
+      <c r="H16" s="35">
+        <v>280858</v>
+      </c>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="7">
@@ -8167,9 +8340,11 @@
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>2000</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="11"/>
+      <c r="C17" s="35">
+        <v>1124549</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="7">
         <v>0.2</v>
       </c>
@@ -8177,8 +8352,10 @@
         <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>2000</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="14"/>
+      <c r="H17" s="35">
+        <v>812573</v>
+      </c>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="7">
@@ -8188,9 +8365,11 @@
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="11"/>
+      <c r="C18" s="35">
+        <v>2489934</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="7">
         <v>0.3</v>
       </c>
@@ -8198,8 +8377,10 @@
         <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="14"/>
+      <c r="H18" s="35">
+        <v>2112914</v>
+      </c>
+      <c r="I18" s="13"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="7">
@@ -8209,9 +8390,11 @@
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>5000</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="11"/>
+      <c r="C19" s="35">
+        <v>7000043</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="7">
         <v>0.5</v>
       </c>
@@ -8219,8 +8402,10 @@
         <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>5000</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="14"/>
+      <c r="H19" s="35">
+        <v>5762327</v>
+      </c>
+      <c r="I19" s="13"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="7">
@@ -8230,9 +8415,11 @@
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="11"/>
+      <c r="C20" s="35">
+        <v>29702695</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="7">
         <v>0.8</v>
       </c>
@@ -8240,10 +8427,12 @@
         <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="14"/>
+      <c r="H20" s="35">
+        <v>16584472</v>
+      </c>
+      <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1">
+    <row r="21" spans="1:9" ht="15" thickBot="1">
       <c r="A21" s="8">
         <v>1</v>
       </c>
@@ -8251,9 +8440,11 @@
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="11"/>
+      <c r="C21" s="36">
+        <v>40013216</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="8">
         <v>1</v>
       </c>
@@ -8261,19 +8452,21 @@
         <f>Table134[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="15"/>
+      <c r="H21" s="36">
+        <v>31087177</v>
+      </c>
+      <c r="I21" s="14"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1"/>
+    <row r="22" spans="1:9" ht="15" thickBot="1"/>
     <row r="23" spans="1:9">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="36"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="34"/>
     </row>
-    <row r="24" spans="1:9" ht="30">
+    <row r="24" spans="1:9" ht="28">
       <c r="A24" s="6" t="s">
         <v>0</v>
       </c>
@@ -8283,7 +8476,7 @@
       <c r="C24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8295,8 +8488,10 @@
         <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="14"/>
+      <c r="C25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="7">
@@ -8306,8 +8501,10 @@
         <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>500</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="14"/>
+      <c r="C26" s="35">
+        <v>88084</v>
+      </c>
+      <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="7">
@@ -8317,8 +8514,10 @@
         <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="14"/>
+      <c r="C27" s="35">
+        <v>237313</v>
+      </c>
+      <c r="D27" s="13"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="7">
@@ -8328,8 +8527,10 @@
         <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>2000</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="14"/>
+      <c r="C28" s="35">
+        <v>739908</v>
+      </c>
+      <c r="D28" s="13"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="7">
@@ -8339,8 +8540,10 @@
         <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="14"/>
+      <c r="C29" s="35">
+        <v>1798397</v>
+      </c>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="7">
@@ -8350,8 +8553,10 @@
         <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>5000</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="14"/>
+      <c r="C30" s="35">
+        <v>6214284</v>
+      </c>
+      <c r="D30" s="13"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="7">
@@ -8361,10 +8566,12 @@
         <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="14"/>
+      <c r="C31" s="35">
+        <v>16625954</v>
+      </c>
+      <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1">
+    <row r="32" spans="1:9" ht="15" thickBot="1">
       <c r="A32" s="8">
         <v>1</v>
       </c>
@@ -8372,8 +8579,10 @@
         <f>Table135[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="15"/>
+      <c r="C32" s="36">
+        <v>31445595</v>
+      </c>
+      <c r="D32" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -8395,15 +8604,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
@@ -8514,6 +8714,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8766,14 +8975,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -8786,6 +8987,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>